<commit_message>
update metadata for Belarus
</commit_message>
<xml_diff>
--- a/inputs/meta.xlsx
+++ b/inputs/meta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/computer/GitHub/fieldmaps/admin-boundaries/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C183D6-1D8E-C442-97F0-4D43E3943B8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D1F440-A969-7F4A-AA43-038027C3F024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2647,8 +2647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U331"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A203" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M243" sqref="M243"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P60" sqref="P60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3336,9 +3336,6 @@
         <v>20</v>
       </c>
       <c r="O41">
-        <v>1</v>
-      </c>
-      <c r="P41">
         <v>2</v>
       </c>
       <c r="Q41">
@@ -3717,9 +3714,6 @@
       </c>
       <c r="O60">
         <v>2</v>
-      </c>
-      <c r="P60">
-        <v>3</v>
       </c>
       <c r="Q60">
         <v>2</v>

</xml_diff>